<commit_message>
export excel of expense data
</commit_message>
<xml_diff>
--- a/document/excel/A1.xlsx
+++ b/document/excel/A1.xlsx
@@ -110,6 +110,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -118,9 +121,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -419,7 +419,7 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -437,26 +437,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.6" customHeight="1">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="2"/>
@@ -468,15 +468,15 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:12" ht="17.399999999999999">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -484,22 +484,22 @@
       <c r="L4" s="3"/>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="7"/>
+      <c r="B6" s="4"/>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="7"/>
+      <c r="B7" s="4"/>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="7"/>
+      <c r="B8" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Fix bug print document
</commit_message>
<xml_diff>
--- a/document/excel/A1.xlsx
+++ b/document/excel/A1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -103,24 +103,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -416,58 +417,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.77734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="23.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15" style="1" customWidth="1"/>
-    <col min="8" max="9" width="10.109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.109375" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="7.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="16" style="2" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="15" style="2" customWidth="1"/>
+    <col min="8" max="9" width="10.140625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.6" customHeight="1">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:7" ht="15.6" customHeight="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="A2" s="7" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:12" ht="17.399999999999999">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:7" ht="18.75">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -477,29 +478,24 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="4" t="s">
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="4"/>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="4" t="s">
+      <c r="B6" s="6"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="4"/>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="4" t="s">
+      <c r="B7" s="6"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="4"/>
+      <c r="B8" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -511,7 +507,7 @@
     <mergeCell ref="A7:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -521,7 +517,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -533,7 +529,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>